<commit_message>
Train and web data concatenated
</commit_message>
<xml_diff>
--- a/KupiPai/KupiPai_log.xlsx
+++ b/KupiPai/KupiPai_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asolo\MyDocs\Personal Docs\DataScience\MyProjects\KupiPai\KupiPai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5DE6600-3DD5-4CFD-8179-5302CDC99BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D6CBC7-26E7-4C8B-9FF8-C7B0CDC53B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Implement UI elements for all the features in Streamlit</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Replaced cadastre feature with region_id and uploaded to the repo</t>
   </si>
@@ -38,6 +35,15 @@
   </si>
   <si>
     <t>Think what to do with owner edrpous</t>
+  </si>
+  <si>
+    <t>Implement prediction with streamlit</t>
+  </si>
+  <si>
+    <t>Read features from Webapp to dataframe and concatenated two dataframes labelling them 1 for training and 0 for validation</t>
+  </si>
+  <si>
+    <t>Process all data n concatenated dataframe to get a normalized result</t>
   </si>
 </sst>
 </file>
@@ -359,13 +365,13 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.21875" customWidth="1"/>
-    <col min="2" max="2" width="94" customWidth="1"/>
+    <col min="2" max="2" width="109.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -373,11 +379,16 @@
         <v>44626</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1">
+        <v>44639</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -386,10 +397,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{738FC74D-B9F4-4F1E-BC9B-A8C126BB5EF3}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -399,17 +410,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First version of Streamlit Webapp completed
</commit_message>
<xml_diff>
--- a/KupiPai/KupiPai_log.xlsx
+++ b/KupiPai/KupiPai_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asolo\MyDocs\Personal Docs\DataScience\MyProjects\KupiPai\KupiPai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D6CBC7-26E7-4C8B-9FF8-C7B0CDC53B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF13D33-F886-466A-8666-D191092699DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,13 +37,13 @@
     <t>Think what to do with owner edrpous</t>
   </si>
   <si>
-    <t>Implement prediction with streamlit</t>
-  </si>
-  <si>
     <t>Read features from Webapp to dataframe and concatenated two dataframes labelling them 1 for training and 0 for validation</t>
   </si>
   <si>
-    <t>Process all data n concatenated dataframe to get a normalized result</t>
+    <t xml:space="preserve">Finished with transferring model from Jupyter notebook to Streamit web app. </t>
+  </si>
+  <si>
+    <t>Check if streamlit web app works correclty in the real time on an existing lot</t>
   </si>
 </sst>
 </file>
@@ -362,10 +362,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -387,6 +387,14 @@
         <v>44639</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>44640</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -397,10 +405,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{738FC74D-B9F4-4F1E-BC9B-A8C126BB5EF3}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -415,16 +423,11 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Replaced outliers with median values
</commit_message>
<xml_diff>
--- a/KupiPai/KupiPai_log.xlsx
+++ b/KupiPai/KupiPai_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asolo\MyDocs\Personal Docs\DataScience\MyProjects\KupiPai\KupiPai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF13D33-F886-466A-8666-D191092699DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC65F3AF-5493-46FF-9C45-1015572D5869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,9 +31,6 @@
     <t>Replaced cadastre feature with region_id and uploaded to the repo</t>
   </si>
   <si>
-    <t>Work with outliers of the numerical features (pricePerOne, estimatedPrice, etc)</t>
-  </si>
-  <si>
     <t>Think what to do with owner edrpous</t>
   </si>
   <si>
@@ -43,7 +40,11 @@
     <t xml:space="preserve">Finished with transferring model from Jupyter notebook to Streamit web app. </t>
   </si>
   <si>
-    <t>Check if streamlit web app works correclty in the real time on an existing lot</t>
+    <t>Replaced outliers with median values for the features which improved slightly the score
+Checked the accuracy of the prediction using the real samples. Works fine</t>
+  </si>
+  <si>
+    <t>Check what is wrong with estinmatedPrice it looks like the range is incorrect in streamlit slider</t>
   </si>
 </sst>
 </file>
@@ -79,9 +80,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B8" sqref="B7:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -387,7 +391,7 @@
         <v>44639</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -395,6 +399,14 @@
         <v>44640</v>
       </c>
       <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>44646</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -405,30 +417,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{738FC74D-B9F4-4F1E-BC9B-A8C126BB5EF3}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A2:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="66.6640625" customWidth="1"/>
+    <col min="1" max="1" width="77.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-    </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed few streamlit sliders to number inputs
</commit_message>
<xml_diff>
--- a/KupiPai/KupiPai_log.xlsx
+++ b/KupiPai/KupiPai_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asolo\MyDocs\Personal Docs\DataScience\MyProjects\KupiPai\KupiPai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC65F3AF-5493-46FF-9C45-1015572D5869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B89A71-4718-4D2A-AD76-36B1F60CC6CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Replaced cadastre feature with region_id and uploaded to the repo</t>
   </si>
@@ -44,7 +44,10 @@
 Checked the accuracy of the prediction using the real samples. Works fine</t>
   </si>
   <si>
-    <t>Check what is wrong with estinmatedPrice it looks like the range is incorrect in streamlit slider</t>
+    <t>Changed some streamlit sliders to input fields</t>
+  </si>
+  <si>
+    <t>Investigate how to depliy streamlit prototype to AWS</t>
   </si>
 </sst>
 </file>
@@ -366,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B7:B8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -410,6 +413,14 @@
         <v>4</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>44647</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -417,10 +428,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{738FC74D-B9F4-4F1E-BC9B-A8C126BB5EF3}">
-  <dimension ref="A2:A3"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -428,13 +439,13 @@
     <col min="1" max="1" width="77.33203125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added a README file with the project description
</commit_message>
<xml_diff>
--- a/KupiPai/KupiPai_log.xlsx
+++ b/KupiPai/KupiPai_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asolo\MyDocs\Personal Docs\DataScience\MyProjects\KupiPai\KupiPai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B89A71-4718-4D2A-AD76-36B1F60CC6CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE27E4C5-3AB4-4916-A19A-843DBF7E4ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,12 +26,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Replaced cadastre feature with region_id and uploaded to the repo</t>
-  </si>
-  <si>
-    <t>Think what to do with owner edrpous</t>
   </si>
   <si>
     <t>Read features from Webapp to dataframe and concatenated two dataframes labelling them 1 for training and 0 for validation</t>
@@ -49,15 +46,32 @@
   <si>
     <t>Investigate how to depliy streamlit prototype to AWS</t>
   </si>
+  <si>
+    <t>https://towardsdatascience.com/how-to-deploy-a-streamlit-app-using-an-amazon-free-ec2-instance-416a41f69dc3</t>
+  </si>
+  <si>
+    <t>How to update model with the new data</t>
+  </si>
+  <si>
+    <t>Code cleanup</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -80,17 +94,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -394,7 +411,7 @@
         <v>44639</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -402,7 +419,7 @@
         <v>44640</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -410,7 +427,7 @@
         <v>44646</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -418,7 +435,7 @@
         <v>44647</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -428,28 +445,41 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{738FC74D-B9F4-4F1E-BC9B-A8C126BB5EF3}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="77.33203125" customWidth="1"/>
+    <col min="1" max="1" width="51.33203125" customWidth="1"/>
+    <col min="2" max="2" width="96.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{4E6CE3AF-098A-4C78-A1A4-680A60CFF03E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cleaned up and styled streamlit app
</commit_message>
<xml_diff>
--- a/KupiPai/KupiPai_log.xlsx
+++ b/KupiPai/KupiPai_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asolo\MyDocs\Personal Docs\DataScience\MyProjects\KupiPai\KupiPai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D4F507-104F-4F38-AE75-20F07F220124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA31795D-4795-416D-B628-D9259446DAE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Replaced cadastre feature with region_id and uploaded to the repo</t>
   </si>
@@ -58,16 +58,13 @@
 Figured out that when you stopping the instance, the IP address on the instance is changed, though the files remain there</t>
   </si>
   <si>
-    <t>Uploaded the app to the AWS EC2 and checked that it is working.</t>
-  </si>
-  <si>
     <t>Uploading Streamlit app to AWS</t>
   </si>
   <si>
-    <t>Remove duplicates for koaatuu locations</t>
-  </si>
-  <si>
-    <t>How to make the streamlit app always running</t>
+    <t>Uploaded the app to the AWS EC2 and checked that it is working. The external IP address is http://18.117.238.29:8501/</t>
+  </si>
+  <si>
+    <t>Read about TMUX</t>
   </si>
 </sst>
 </file>
@@ -405,7 +402,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -467,7 +464,7 @@
         <v>44654</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -477,48 +474,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{738FC74D-B9F4-4F1E-BC9B-A8C126BB5EF3}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="57.6640625" customWidth="1"/>
-    <col min="2" max="2" width="96.5546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="107.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" xr:uid="{C08354DE-1059-4DAA-B97F-FF51B51CD8AC}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -538,7 +524,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
KupiPai project cleaned up
</commit_message>
<xml_diff>
--- a/KupiPai/KupiPai_log.xlsx
+++ b/KupiPai/KupiPai_log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asolo\MyDocs\Personal Docs\DataScience\MyProjects\KupiPai\KupiPai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA31795D-4795-416D-B628-D9259446DAE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1083914F-0F96-497F-BAF8-6FEF6C980296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Replaced cadastre feature with region_id and uploaded to the repo</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>Read about TMUX</t>
+  </si>
+  <si>
+    <t>Try Lasso selection for the features</t>
   </si>
 </sst>
 </file>
@@ -401,8 +404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -474,10 +477,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{738FC74D-B9F4-4F1E-BC9B-A8C126BB5EF3}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -499,6 +502,12 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>